<commit_message>
added new info column
</commit_message>
<xml_diff>
--- a/potato_iformation.xlsx
+++ b/potato_iformation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\Potato_chips\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57564C0C-CB77-49E6-A1FB-53F58B5B50B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34450F13-1C70-4F0B-9CF1-B3A21106D3C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="314">
   <si>
     <t>1.1</t>
   </si>
@@ -970,6 +970,12 @@
   </si>
   <si>
     <t>numbers</t>
+  </si>
+  <si>
+    <t>anthocyanin_stem</t>
+  </si>
+  <si>
+    <t>anthocyanin_leaf</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1284,6 +1290,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1564,11 +1571,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y296"/>
+  <dimension ref="A1:Z296"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H279" sqref="H279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1589,7 +1596,7 @@
     <col min="24" max="24" width="8.7265625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="6" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" s="6" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>311</v>
       </c>
@@ -1662,9 +1669,14 @@
       <c r="X1" s="48" t="s">
         <v>310</v>
       </c>
-      <c r="Y1" s="26"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y1" s="26" t="s">
+        <v>312</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1728,9 +1740,14 @@
       <c r="X2" s="14">
         <v>54</v>
       </c>
-      <c r="Y2" s="20"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y2" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1792,9 +1809,14 @@
       <c r="X3" s="14">
         <v>86</v>
       </c>
-      <c r="Y3" s="20"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y3" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1863,9 +1885,14 @@
       <c r="X4" s="14">
         <v>56</v>
       </c>
-      <c r="Y4" s="20"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y4" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1929,9 +1956,14 @@
       <c r="X5" s="14">
         <v>168</v>
       </c>
-      <c r="Y5" s="20"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y5" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2005,7 +2037,7 @@
       </c>
       <c r="Y6" s="20"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2082,9 +2114,14 @@
       <c r="X7" s="14">
         <v>132</v>
       </c>
-      <c r="Y7" s="20"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y7" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -2161,9 +2198,14 @@
       <c r="X8" s="14">
         <v>10</v>
       </c>
-      <c r="Y8" s="20"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y8" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -2240,9 +2282,14 @@
       <c r="X9" s="14">
         <v>134</v>
       </c>
-      <c r="Y9" s="20"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y9" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2314,9 +2361,14 @@
       <c r="X10" s="14">
         <v>140</v>
       </c>
-      <c r="Y10" s="20"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y10" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2380,9 +2432,14 @@
       <c r="X11" s="14">
         <v>114</v>
       </c>
-      <c r="Y11" s="20"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y11" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2459,9 +2516,14 @@
       <c r="X12" s="14">
         <v>74</v>
       </c>
-      <c r="Y12" s="20"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y12" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2528,9 +2590,14 @@
       <c r="X13" s="14">
         <v>52</v>
       </c>
-      <c r="Y13" s="20"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y13" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2594,9 +2661,14 @@
       <c r="X14" s="14">
         <v>112</v>
       </c>
-      <c r="Y14" s="20"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y14" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2660,9 +2732,14 @@
       <c r="X15" s="14">
         <v>136</v>
       </c>
-      <c r="Y15" s="20"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y15" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -2726,9 +2803,14 @@
       <c r="X16" s="14">
         <v>88</v>
       </c>
-      <c r="Y16" s="20"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y16" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -2800,9 +2882,14 @@
       <c r="X17" s="14">
         <v>24</v>
       </c>
-      <c r="Y17" s="20"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y17" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -2874,9 +2961,14 @@
       <c r="X18" s="14">
         <v>80</v>
       </c>
-      <c r="Y18" s="20"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y18" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -2948,9 +3040,14 @@
       <c r="X19" s="14">
         <v>82</v>
       </c>
-      <c r="Y19" s="20"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y19" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -3022,9 +3119,14 @@
       <c r="X20" s="14">
         <v>86</v>
       </c>
-      <c r="Y20" s="20"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y20" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -3096,9 +3198,14 @@
       <c r="X21" s="14">
         <v>66</v>
       </c>
-      <c r="Y21" s="20"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y21" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -3170,9 +3277,14 @@
       <c r="X22" s="14">
         <v>84</v>
       </c>
-      <c r="Y22" s="20"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y22" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
@@ -3241,9 +3353,14 @@
       <c r="X23" s="14">
         <v>124</v>
       </c>
-      <c r="Y23" s="20"/>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y23" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
@@ -3320,9 +3437,14 @@
       <c r="X24" s="14">
         <v>140</v>
       </c>
-      <c r="Y24" s="20"/>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y24" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -3386,9 +3508,14 @@
       <c r="X25" s="14">
         <v>112</v>
       </c>
-      <c r="Y25" s="20"/>
-    </row>
-    <row r="26" spans="1:25" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y25" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
@@ -3465,9 +3592,14 @@
       <c r="X26" s="14">
         <v>120</v>
       </c>
-      <c r="Y26" s="20"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y26" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
@@ -3536,9 +3668,14 @@
       <c r="X27" s="14">
         <v>140</v>
       </c>
-      <c r="Y27" s="20"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y27" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
@@ -3602,9 +3739,14 @@
       <c r="X28" s="14">
         <v>154</v>
       </c>
-      <c r="Y28" s="20"/>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y28" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -3676,9 +3818,14 @@
       <c r="X29" s="14">
         <v>134</v>
       </c>
-      <c r="Y29" s="20"/>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y29" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -3742,9 +3889,14 @@
       <c r="X30" s="14">
         <v>122</v>
       </c>
-      <c r="Y30" s="20"/>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y30" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -3813,9 +3965,14 @@
       <c r="X31" s="14">
         <v>136</v>
       </c>
-      <c r="Y31" s="20"/>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y31" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -3892,9 +4049,14 @@
       <c r="X32" s="14">
         <v>110</v>
       </c>
-      <c r="Y32" s="20"/>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y32" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -3966,9 +4128,14 @@
       <c r="X33" s="14">
         <v>78</v>
       </c>
-      <c r="Y33" s="20"/>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y33" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -4032,9 +4199,14 @@
       <c r="X34" s="14">
         <v>80</v>
       </c>
-      <c r="Y34" s="20"/>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y34" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>274</v>
       </c>
@@ -4082,7 +4254,7 @@
       <c r="W35" s="18"/>
       <c r="Y35" s="20"/>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>275</v>
       </c>
@@ -4130,7 +4302,7 @@
       <c r="W36" s="18"/>
       <c r="Y36" s="20"/>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>33</v>
       </c>
@@ -4199,9 +4371,14 @@
       <c r="X37" s="14">
         <v>172</v>
       </c>
-      <c r="Y37" s="20"/>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y37" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>34</v>
       </c>
@@ -4265,9 +4442,14 @@
       <c r="X38" s="14">
         <v>106</v>
       </c>
-      <c r="Y38" s="20"/>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y38" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
@@ -4336,9 +4518,14 @@
       <c r="X39" s="14">
         <v>132</v>
       </c>
-      <c r="Y39" s="20"/>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y39" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>36</v>
       </c>
@@ -4402,9 +4589,14 @@
       <c r="X40" s="14">
         <v>182</v>
       </c>
-      <c r="Y40" s="20"/>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y40" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>37</v>
       </c>
@@ -4473,9 +4665,14 @@
       <c r="X41" s="14">
         <v>50</v>
       </c>
-      <c r="Y41" s="20"/>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y41" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>38</v>
       </c>
@@ -4539,9 +4736,14 @@
       <c r="X42" s="14">
         <v>54</v>
       </c>
-      <c r="Y42" s="20"/>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y42" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>39</v>
       </c>
@@ -4605,9 +4807,14 @@
       <c r="X43" s="14">
         <v>54</v>
       </c>
-      <c r="Y43" s="20"/>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y43" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>40</v>
       </c>
@@ -4671,9 +4878,14 @@
       <c r="X44" s="14">
         <v>36</v>
       </c>
-      <c r="Y44" s="20"/>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y44" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>41</v>
       </c>
@@ -4703,7 +4915,7 @@
       <c r="W45" s="18"/>
       <c r="Y45" s="20"/>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>42</v>
       </c>
@@ -4767,9 +4979,14 @@
       <c r="X46" s="14">
         <v>50</v>
       </c>
-      <c r="Y46" s="20"/>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y46" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>43</v>
       </c>
@@ -4841,9 +5058,14 @@
       <c r="X47" s="14">
         <v>100</v>
       </c>
-      <c r="Y47" s="20"/>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y47" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>44</v>
       </c>
@@ -4915,9 +5137,14 @@
       <c r="X48" s="14">
         <v>152</v>
       </c>
-      <c r="Y48" s="20"/>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y48" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>45</v>
       </c>
@@ -4989,9 +5216,14 @@
       <c r="X49" s="14">
         <v>142</v>
       </c>
-      <c r="Y49" s="20"/>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y49" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>276</v>
       </c>
@@ -5039,7 +5271,7 @@
       <c r="W50" s="18"/>
       <c r="Y50" s="20"/>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>46</v>
       </c>
@@ -5111,9 +5343,14 @@
       <c r="X51" s="14">
         <v>138</v>
       </c>
-      <c r="Y51" s="20"/>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y51" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
         <v>277</v>
       </c>
@@ -5161,7 +5398,7 @@
       <c r="W52" s="18"/>
       <c r="Y52" s="20"/>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>47</v>
       </c>
@@ -5233,9 +5470,14 @@
       <c r="X53" s="14">
         <v>100</v>
       </c>
-      <c r="Y53" s="20"/>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y53" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>48</v>
       </c>
@@ -5299,9 +5541,14 @@
       <c r="X54" s="14">
         <v>116</v>
       </c>
-      <c r="Y54" s="20"/>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y54" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>49</v>
       </c>
@@ -5365,9 +5612,14 @@
       <c r="X55" s="14">
         <v>88</v>
       </c>
-      <c r="Y55" s="20"/>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y55" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>50</v>
       </c>
@@ -5431,9 +5683,14 @@
       <c r="X56" s="14">
         <v>112</v>
       </c>
-      <c r="Y56" s="20"/>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y56" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>51</v>
       </c>
@@ -5505,9 +5762,14 @@
       <c r="X57" s="14">
         <v>90</v>
       </c>
-      <c r="Y57" s="20"/>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y57" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>52</v>
       </c>
@@ -5571,9 +5833,14 @@
       <c r="X58" s="14">
         <v>96</v>
       </c>
-      <c r="Y58" s="20"/>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y58" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>53</v>
       </c>
@@ -5645,9 +5912,14 @@
       <c r="X59" s="14">
         <v>94</v>
       </c>
-      <c r="Y59" s="20"/>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y59" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>54</v>
       </c>
@@ -5719,9 +5991,14 @@
       <c r="X60" s="14">
         <v>96</v>
       </c>
-      <c r="Y60" s="20"/>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y60" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>55</v>
       </c>
@@ -5793,9 +6070,14 @@
       <c r="X61" s="14">
         <v>106</v>
       </c>
-      <c r="Y61" s="20"/>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y61" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>287</v>
       </c>
@@ -5867,9 +6149,14 @@
       <c r="X62" s="14">
         <v>66</v>
       </c>
-      <c r="Y62" s="20"/>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y62" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>56</v>
       </c>
@@ -5933,9 +6220,14 @@
       <c r="X63" s="14">
         <v>98</v>
       </c>
-      <c r="Y63" s="20"/>
-    </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y63" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>286</v>
       </c>
@@ -6007,9 +6299,14 @@
       <c r="X64" s="14">
         <v>38</v>
       </c>
-      <c r="Y64" s="20"/>
-    </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y64" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>57</v>
       </c>
@@ -6081,9 +6378,14 @@
       <c r="X65" s="14">
         <v>68</v>
       </c>
-      <c r="Y65" s="20"/>
-    </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y65" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>58</v>
       </c>
@@ -6160,9 +6462,14 @@
       <c r="X66" s="14">
         <v>68</v>
       </c>
-      <c r="Y66" s="20"/>
-    </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y66" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>59</v>
       </c>
@@ -6226,9 +6533,14 @@
       <c r="X67" s="14">
         <v>66</v>
       </c>
-      <c r="Y67" s="20"/>
-    </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y67" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>60</v>
       </c>
@@ -6292,9 +6604,14 @@
       <c r="X68" s="14">
         <v>116</v>
       </c>
-      <c r="Y68" s="20"/>
-    </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y68" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>61</v>
       </c>
@@ -6358,9 +6675,14 @@
       <c r="X69" s="14">
         <v>128</v>
       </c>
-      <c r="Y69" s="20"/>
-    </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y69" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>62</v>
       </c>
@@ -6424,9 +6746,14 @@
       <c r="X70" s="14">
         <v>102</v>
       </c>
-      <c r="Y70" s="20"/>
-    </row>
-    <row r="71" spans="1:25" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y70" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:26" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>63</v>
       </c>
@@ -6490,9 +6817,14 @@
       <c r="X71" s="14">
         <v>74</v>
       </c>
-      <c r="Y71" s="20"/>
-    </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y71" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>64</v>
       </c>
@@ -6564,9 +6896,14 @@
       <c r="X72" s="14">
         <v>90</v>
       </c>
-      <c r="Y72" s="20"/>
-    </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y72" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>65</v>
       </c>
@@ -6638,9 +6975,14 @@
       <c r="X73" s="14">
         <v>104</v>
       </c>
-      <c r="Y73" s="20"/>
-    </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y73" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
         <v>66</v>
       </c>
@@ -6712,9 +7054,14 @@
       <c r="X74" s="14">
         <v>88</v>
       </c>
-      <c r="Y74" s="20"/>
-    </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y74" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A75" s="4" t="s">
         <v>67</v>
       </c>
@@ -6776,9 +7123,14 @@
       <c r="X75" s="14">
         <v>102</v>
       </c>
-      <c r="Y75" s="20"/>
-    </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y75" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
         <v>68</v>
       </c>
@@ -6842,9 +7194,14 @@
       <c r="X76" s="14">
         <v>26</v>
       </c>
-      <c r="Y76" s="20"/>
-    </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y76" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>69</v>
       </c>
@@ -6921,9 +7278,14 @@
       <c r="X77" s="14">
         <v>124</v>
       </c>
-      <c r="Y77" s="20"/>
-    </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y77" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>70</v>
       </c>
@@ -6995,9 +7357,14 @@
       <c r="X78" s="14">
         <v>120</v>
       </c>
-      <c r="Y78" s="20"/>
-    </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y78" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>71</v>
       </c>
@@ -7061,9 +7428,14 @@
       <c r="X79" s="14">
         <v>130</v>
       </c>
-      <c r="Y79" s="20"/>
-    </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y79" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>72</v>
       </c>
@@ -7140,9 +7512,14 @@
       <c r="X80" s="14">
         <v>90</v>
       </c>
-      <c r="Y80" s="20"/>
-    </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y80" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>73</v>
       </c>
@@ -7211,9 +7588,14 @@
       <c r="X81" s="14">
         <v>108</v>
       </c>
-      <c r="Y81" s="20"/>
-    </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y81" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>74</v>
       </c>
@@ -7285,9 +7667,14 @@
       <c r="X82" s="14">
         <v>108</v>
       </c>
-      <c r="Y82" s="20"/>
-    </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y82" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>75</v>
       </c>
@@ -7356,9 +7743,14 @@
       <c r="X83" s="14">
         <v>138</v>
       </c>
-      <c r="Y83" s="20"/>
-    </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y83" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>76</v>
       </c>
@@ -7422,9 +7814,14 @@
       <c r="X84" s="14">
         <v>116</v>
       </c>
-      <c r="Y84" s="20"/>
-    </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y84" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>77</v>
       </c>
@@ -7496,9 +7893,14 @@
       <c r="X85" s="14">
         <v>98</v>
       </c>
-      <c r="Y85" s="20"/>
-    </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y85" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>78</v>
       </c>
@@ -7575,9 +7977,14 @@
       <c r="X86" s="14">
         <v>106</v>
       </c>
-      <c r="Y86" s="20"/>
-    </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y86" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>79</v>
       </c>
@@ -7649,9 +8056,14 @@
       <c r="X87" s="14">
         <v>132</v>
       </c>
-      <c r="Y87" s="20"/>
-    </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y87" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>80</v>
       </c>
@@ -7728,9 +8140,14 @@
       <c r="X88" s="14">
         <v>102</v>
       </c>
-      <c r="Y88" s="20"/>
-    </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y88" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>81</v>
       </c>
@@ -7794,9 +8211,14 @@
       <c r="X89" s="14">
         <v>56</v>
       </c>
-      <c r="Y89" s="20"/>
-    </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y89" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>82</v>
       </c>
@@ -7868,9 +8290,14 @@
       <c r="X90" s="14">
         <v>124</v>
       </c>
-      <c r="Y90" s="20"/>
-    </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y90" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
         <v>278</v>
       </c>
@@ -7918,7 +8345,7 @@
       <c r="W91" s="18"/>
       <c r="Y91" s="20"/>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A92" s="7" t="s">
         <v>83</v>
       </c>
@@ -7974,9 +8401,14 @@
       <c r="X92" s="14">
         <v>0.3</v>
       </c>
-      <c r="Y92" s="20"/>
-    </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y92" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>84</v>
       </c>
@@ -8038,9 +8470,14 @@
       <c r="X93" s="14">
         <v>2.2000000000000002</v>
       </c>
-      <c r="Y93" s="20"/>
-    </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y93" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>85</v>
       </c>
@@ -8087,7 +8524,7 @@
       <c r="W94" s="18"/>
       <c r="Y94" s="20"/>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>86</v>
       </c>
@@ -8135,7 +8572,7 @@
       <c r="W95" s="18"/>
       <c r="Y95" s="20"/>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>87</v>
       </c>
@@ -8175,7 +8612,7 @@
       <c r="W96" s="18"/>
       <c r="Y96" s="20"/>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>88</v>
       </c>
@@ -8244,9 +8681,14 @@
       <c r="X97" s="14">
         <v>130</v>
       </c>
-      <c r="Y97" s="20"/>
-    </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y97" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>89</v>
       </c>
@@ -8318,9 +8760,14 @@
       <c r="X98" s="14">
         <v>128</v>
       </c>
-      <c r="Y98" s="20"/>
-    </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y98" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>90</v>
       </c>
@@ -8392,9 +8839,14 @@
       <c r="X99" s="14">
         <v>98</v>
       </c>
-      <c r="Y99" s="20"/>
-    </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y99" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>91</v>
       </c>
@@ -8458,9 +8910,14 @@
       <c r="X100" s="14">
         <v>124</v>
       </c>
-      <c r="Y100" s="20"/>
-    </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y100" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>92</v>
       </c>
@@ -8537,9 +8994,14 @@
       <c r="X101" s="14">
         <v>86</v>
       </c>
-      <c r="Y101" s="20"/>
-    </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y101" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>93</v>
       </c>
@@ -8611,9 +9073,14 @@
       <c r="X102" s="14">
         <v>126</v>
       </c>
-      <c r="Y102" s="20"/>
-    </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y102" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>94</v>
       </c>
@@ -8685,9 +9152,14 @@
       <c r="X103" s="14">
         <v>120</v>
       </c>
-      <c r="Y103" s="20"/>
-    </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y103" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>95</v>
       </c>
@@ -8764,9 +9236,14 @@
       <c r="X104" s="14">
         <v>130</v>
       </c>
-      <c r="Y104" s="20"/>
-    </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y104" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>96</v>
       </c>
@@ -8838,9 +9315,14 @@
       <c r="X105" s="14">
         <v>120</v>
       </c>
-      <c r="Y105" s="20"/>
-    </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y105" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>97</v>
       </c>
@@ -8912,9 +9394,14 @@
       <c r="X106" s="14">
         <v>92</v>
       </c>
-      <c r="Y106" s="20"/>
-    </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y106" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>279</v>
       </c>
@@ -8962,7 +9449,7 @@
       <c r="W107" s="18"/>
       <c r="Y107" s="20"/>
     </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
         <v>98</v>
       </c>
@@ -9034,9 +9521,14 @@
       <c r="X108" s="14">
         <v>88</v>
       </c>
-      <c r="Y108" s="20"/>
-    </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y108" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
         <v>280</v>
       </c>
@@ -9084,7 +9576,7 @@
       <c r="W109" s="18"/>
       <c r="Y109" s="20"/>
     </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>99</v>
       </c>
@@ -9154,9 +9646,14 @@
       <c r="X110" s="14">
         <v>80</v>
       </c>
-      <c r="Y110" s="20"/>
-    </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y110" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>100</v>
       </c>
@@ -9228,9 +9725,14 @@
       <c r="X111" s="14">
         <v>106</v>
       </c>
-      <c r="Y111" s="20"/>
-    </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y111" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>101</v>
       </c>
@@ -9302,9 +9804,14 @@
       <c r="X112" s="14">
         <v>132</v>
       </c>
-      <c r="Y112" s="20"/>
-    </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y112" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>102</v>
       </c>
@@ -9368,9 +9875,14 @@
       <c r="X113" s="14">
         <v>70</v>
       </c>
-      <c r="Y113" s="20"/>
-    </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y113" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
         <v>103</v>
       </c>
@@ -9442,9 +9954,14 @@
       <c r="X114" s="14">
         <v>78</v>
       </c>
-      <c r="Y114" s="20"/>
-    </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y114" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>104</v>
       </c>
@@ -9516,9 +10033,14 @@
       <c r="X115" s="14">
         <v>110</v>
       </c>
-      <c r="Y115" s="20"/>
-    </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y115" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A116" s="3" t="s">
         <v>105</v>
       </c>
@@ -9582,9 +10104,14 @@
       <c r="X116" s="14">
         <v>36</v>
       </c>
-      <c r="Y116" s="20"/>
-    </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y116" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A117" s="3" t="s">
         <v>106</v>
       </c>
@@ -9659,9 +10186,14 @@
       <c r="X117" s="14">
         <v>120</v>
       </c>
-      <c r="Y117" s="20"/>
-    </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y117" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="s">
         <v>107</v>
       </c>
@@ -9733,9 +10265,14 @@
       <c r="X118" s="14">
         <v>154</v>
       </c>
-      <c r="Y118" s="20"/>
-    </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y118" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A119" s="3" t="s">
         <v>108</v>
       </c>
@@ -9807,9 +10344,14 @@
       <c r="X119" s="14">
         <v>146</v>
       </c>
-      <c r="Y119" s="20"/>
-    </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y119" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="s">
         <v>109</v>
       </c>
@@ -9881,9 +10423,14 @@
       <c r="X120" s="14">
         <v>162</v>
       </c>
-      <c r="Y120" s="20"/>
-    </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y120" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A121" s="3" t="s">
         <v>110</v>
       </c>
@@ -9955,9 +10502,14 @@
       <c r="X121" s="14">
         <v>178</v>
       </c>
-      <c r="Y121" s="20"/>
-    </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y121" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="s">
         <v>281</v>
       </c>
@@ -10005,7 +10557,7 @@
       <c r="W122" s="18"/>
       <c r="Y122" s="20"/>
     </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
         <v>111</v>
       </c>
@@ -10082,9 +10634,14 @@
       <c r="X123" s="14">
         <v>94</v>
       </c>
-      <c r="Y123" s="20"/>
-    </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y123" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="s">
         <v>282</v>
       </c>
@@ -10132,7 +10689,7 @@
       <c r="W124" s="18"/>
       <c r="Y124" s="20"/>
     </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
         <v>112</v>
       </c>
@@ -10209,9 +10766,14 @@
       <c r="X125" s="14">
         <v>84</v>
       </c>
-      <c r="Y125" s="20"/>
-    </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y125" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="s">
         <v>283</v>
       </c>
@@ -10259,7 +10821,7 @@
       <c r="W126" s="18"/>
       <c r="Y126" s="20"/>
     </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>113</v>
       </c>
@@ -10336,9 +10898,14 @@
       <c r="X127" s="14">
         <v>84</v>
       </c>
-      <c r="Y127" s="20"/>
-    </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y127" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
         <v>114</v>
       </c>
@@ -10410,9 +10977,14 @@
       <c r="X128" s="14">
         <v>146</v>
       </c>
-      <c r="Y128" s="20"/>
-    </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y128" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
         <v>115</v>
       </c>
@@ -10489,9 +11061,14 @@
       <c r="X129" s="14">
         <v>160</v>
       </c>
-      <c r="Y129" s="20"/>
-    </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y129" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>116</v>
       </c>
@@ -10563,9 +11140,14 @@
       <c r="X130" s="14">
         <v>126</v>
       </c>
-      <c r="Y130" s="20"/>
-    </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y130" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>117</v>
       </c>
@@ -10642,9 +11224,14 @@
       <c r="X131" s="14">
         <v>120</v>
       </c>
-      <c r="Y131" s="20"/>
-    </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y131" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>118</v>
       </c>
@@ -10714,9 +11301,14 @@
       <c r="X132" s="14">
         <v>140</v>
       </c>
-      <c r="Y132" s="20"/>
-    </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y132" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>119</v>
       </c>
@@ -10788,9 +11380,14 @@
       <c r="X133" s="14">
         <v>140</v>
       </c>
-      <c r="Y133" s="20"/>
-    </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y133" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
         <v>120</v>
       </c>
@@ -10862,9 +11459,14 @@
       <c r="X134" s="14">
         <v>120</v>
       </c>
-      <c r="Y134" s="20"/>
-    </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y134" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
         <v>121</v>
       </c>
@@ -10928,9 +11530,14 @@
       <c r="X135" s="14">
         <v>88</v>
       </c>
-      <c r="Y135" s="20"/>
-    </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y135" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
         <v>122</v>
       </c>
@@ -11002,9 +11609,14 @@
       <c r="X136" s="14">
         <v>106</v>
       </c>
-      <c r="Y136" s="20"/>
-    </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y136" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
         <v>123</v>
       </c>
@@ -11066,9 +11678,14 @@
       <c r="X137" s="14">
         <v>36</v>
       </c>
-      <c r="Y137" s="20"/>
-    </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y137" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
         <v>124</v>
       </c>
@@ -11132,9 +11749,14 @@
       <c r="X138" s="14">
         <v>48</v>
       </c>
-      <c r="Y138" s="20"/>
-    </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y138" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
         <v>125</v>
       </c>
@@ -11206,9 +11828,14 @@
       <c r="X139" s="14">
         <v>76</v>
       </c>
-      <c r="Y139" s="20"/>
-    </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y139" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
         <v>126</v>
       </c>
@@ -11256,7 +11883,7 @@
       <c r="W140" s="18"/>
       <c r="Y140" s="20"/>
     </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
         <v>127</v>
       </c>
@@ -11320,9 +11947,14 @@
       <c r="X141" s="14">
         <v>136</v>
       </c>
-      <c r="Y141" s="20"/>
-    </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y141" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
         <v>128</v>
       </c>
@@ -11370,7 +12002,7 @@
       <c r="W142" s="18"/>
       <c r="Y142" s="20"/>
     </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>129</v>
       </c>
@@ -11447,9 +12079,14 @@
       <c r="X143" s="14">
         <v>68</v>
       </c>
-      <c r="Y143" s="20"/>
-    </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y143" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
         <v>130</v>
       </c>
@@ -11521,9 +12158,14 @@
       <c r="X144" s="14">
         <v>152</v>
       </c>
-      <c r="Y144" s="20"/>
-    </row>
-    <row r="145" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y144" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
         <v>131</v>
       </c>
@@ -11600,9 +12242,14 @@
       <c r="X145" s="14">
         <v>122</v>
       </c>
-      <c r="Y145" s="20"/>
-    </row>
-    <row r="146" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y145" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
         <v>132</v>
       </c>
@@ -11677,9 +12324,14 @@
       <c r="X146" s="14">
         <v>170</v>
       </c>
-      <c r="Y146" s="20"/>
-    </row>
-    <row r="147" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y146" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
         <v>133</v>
       </c>
@@ -11751,9 +12403,14 @@
       <c r="X147" s="14">
         <v>126</v>
       </c>
-      <c r="Y147" s="20"/>
-    </row>
-    <row r="148" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y147" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
         <v>134</v>
       </c>
@@ -11830,9 +12487,14 @@
       <c r="X148" s="14">
         <v>136</v>
       </c>
-      <c r="Y148" s="20"/>
-    </row>
-    <row r="149" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y148" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
         <v>135</v>
       </c>
@@ -11904,9 +12566,14 @@
       <c r="X149" s="14">
         <v>130</v>
       </c>
-      <c r="Y149" s="20"/>
-    </row>
-    <row r="150" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y149" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z149" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
         <v>136</v>
       </c>
@@ -11978,9 +12645,14 @@
       <c r="X150" s="14">
         <v>140</v>
       </c>
-      <c r="Y150" s="20"/>
-    </row>
-    <row r="151" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y150" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z150" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
         <v>137</v>
       </c>
@@ -12044,9 +12716,14 @@
       <c r="X151" s="14">
         <v>130</v>
       </c>
-      <c r="Y151" s="20"/>
-    </row>
-    <row r="152" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y151" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z151" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
         <v>138</v>
       </c>
@@ -12116,9 +12793,14 @@
       <c r="X152" s="14">
         <v>52</v>
       </c>
-      <c r="Y152" s="20"/>
-    </row>
-    <row r="153" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y152" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z152" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
         <v>139</v>
       </c>
@@ -12185,9 +12867,14 @@
       <c r="X153" s="14">
         <v>60</v>
       </c>
-      <c r="Y153" s="20"/>
-    </row>
-    <row r="154" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y153" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z153" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>140</v>
       </c>
@@ -12259,9 +12946,14 @@
       <c r="X154" s="14">
         <v>98</v>
       </c>
-      <c r="Y154" s="20"/>
-    </row>
-    <row r="155" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y154" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z154" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
         <v>141</v>
       </c>
@@ -12325,9 +13017,14 @@
       <c r="X155" s="14">
         <v>40</v>
       </c>
-      <c r="Y155" s="20"/>
-    </row>
-    <row r="156" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y155" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z155" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
         <v>142</v>
       </c>
@@ -12391,9 +13088,14 @@
       <c r="X156" s="14">
         <v>70</v>
       </c>
-      <c r="Y156" s="20"/>
-    </row>
-    <row r="157" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y156" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z156" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
         <v>143</v>
       </c>
@@ -12427,7 +13129,7 @@
       <c r="W157" s="18"/>
       <c r="Y157" s="20"/>
     </row>
-    <row r="158" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
         <v>144</v>
       </c>
@@ -12499,9 +13201,14 @@
       <c r="X158" s="14">
         <v>102</v>
       </c>
-      <c r="Y158" s="20"/>
-    </row>
-    <row r="159" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y158" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z158" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
         <v>145</v>
       </c>
@@ -12578,9 +13285,14 @@
       <c r="X159" s="14">
         <v>124</v>
       </c>
-      <c r="Y159" s="20"/>
-    </row>
-    <row r="160" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y159" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z159" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
         <v>146</v>
       </c>
@@ -12646,7 +13358,7 @@
       </c>
       <c r="Y160" s="20"/>
     </row>
-    <row r="161" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
         <v>147</v>
       </c>
@@ -12707,7 +13419,7 @@
       <c r="W161" s="18"/>
       <c r="Y161" s="20"/>
     </row>
-    <row r="162" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
         <v>148</v>
       </c>
@@ -12769,9 +13481,14 @@
       <c r="X162" s="14">
         <v>0.8</v>
       </c>
-      <c r="Y162" s="20"/>
-    </row>
-    <row r="163" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y162" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z162" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
         <v>149</v>
       </c>
@@ -12843,9 +13560,14 @@
       <c r="X163" s="14">
         <v>7.8</v>
       </c>
-      <c r="Y163" s="20"/>
-    </row>
-    <row r="164" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y163" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z163" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
         <v>150</v>
       </c>
@@ -12909,9 +13631,14 @@
       <c r="X164" s="14">
         <v>36</v>
       </c>
-      <c r="Y164" s="20"/>
-    </row>
-    <row r="165" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y164" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z164" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
         <v>151</v>
       </c>
@@ -12975,7 +13702,7 @@
       </c>
       <c r="Y165" s="20"/>
     </row>
-    <row r="166" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
         <v>152</v>
       </c>
@@ -13044,9 +13771,14 @@
       <c r="X166" s="14">
         <v>2.6</v>
       </c>
-      <c r="Y166" s="20"/>
-    </row>
-    <row r="167" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y166" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z166" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
         <v>153</v>
       </c>
@@ -13118,9 +13850,14 @@
       <c r="X167" s="14">
         <v>112</v>
       </c>
-      <c r="Y167" s="20"/>
-    </row>
-    <row r="168" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y167" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z167" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
         <v>154</v>
       </c>
@@ -13192,9 +13929,14 @@
       <c r="X168" s="14">
         <v>86</v>
       </c>
-      <c r="Y168" s="20"/>
-    </row>
-    <row r="169" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y168" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z168" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
         <v>155</v>
       </c>
@@ -13266,9 +14008,14 @@
       <c r="X169" s="14">
         <v>92</v>
       </c>
-      <c r="Y169" s="20"/>
-    </row>
-    <row r="170" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y169" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z169" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
         <v>156</v>
       </c>
@@ -13340,9 +14087,14 @@
       <c r="X170" s="14">
         <v>72</v>
       </c>
-      <c r="Y170" s="20"/>
-    </row>
-    <row r="171" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y170" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z170" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
         <v>157</v>
       </c>
@@ -13419,9 +14171,14 @@
       <c r="X171" s="14">
         <v>80</v>
       </c>
-      <c r="Y171" s="20"/>
-    </row>
-    <row r="172" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y171" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z171" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
         <v>158</v>
       </c>
@@ -13493,9 +14250,14 @@
       <c r="X172" s="14">
         <v>106</v>
       </c>
-      <c r="Y172" s="20"/>
-    </row>
-    <row r="173" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y172" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z172" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
         <v>284</v>
       </c>
@@ -13545,7 +14307,7 @@
       <c r="W173" s="18"/>
       <c r="Y173" s="20"/>
     </row>
-    <row r="174" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A174" s="2" t="s">
         <v>159</v>
       </c>
@@ -13622,9 +14384,14 @@
       <c r="X174" s="14">
         <v>150</v>
       </c>
-      <c r="Y174" s="20"/>
-    </row>
-    <row r="175" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y174" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z174" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A175" s="2" t="s">
         <v>285</v>
       </c>
@@ -13672,7 +14439,7 @@
       <c r="W175" s="18"/>
       <c r="Y175" s="20"/>
     </row>
-    <row r="176" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
         <v>160</v>
       </c>
@@ -13736,9 +14503,14 @@
       <c r="X176" s="14">
         <v>86</v>
       </c>
-      <c r="Y176" s="20"/>
-    </row>
-    <row r="177" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y176" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
         <v>161</v>
       </c>
@@ -13810,9 +14582,14 @@
       <c r="X177" s="14">
         <v>106</v>
       </c>
-      <c r="Y177" s="20"/>
-    </row>
-    <row r="178" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y177" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
         <v>162</v>
       </c>
@@ -13884,9 +14661,14 @@
       <c r="X178" s="14">
         <v>76</v>
       </c>
-      <c r="Y178" s="20"/>
-    </row>
-    <row r="179" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y178" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A179" s="1" t="s">
         <v>163</v>
       </c>
@@ -13934,7 +14716,7 @@
       <c r="W179" s="18"/>
       <c r="Y179" s="20"/>
     </row>
-    <row r="180" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
         <v>164</v>
       </c>
@@ -13998,9 +14780,14 @@
       <c r="X180" s="14">
         <v>42</v>
       </c>
-      <c r="Y180" s="20"/>
-    </row>
-    <row r="181" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y180" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z180" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A181" s="1" t="s">
         <v>165</v>
       </c>
@@ -14050,7 +14837,7 @@
       <c r="W181" s="18"/>
       <c r="Y181" s="20"/>
     </row>
-    <row r="182" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="s">
         <v>166</v>
       </c>
@@ -14098,7 +14885,7 @@
       <c r="W182" s="18"/>
       <c r="Y182" s="20"/>
     </row>
-    <row r="183" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
         <v>167</v>
       </c>
@@ -14162,9 +14949,14 @@
       <c r="X183" s="14">
         <v>50</v>
       </c>
-      <c r="Y183" s="20"/>
-    </row>
-    <row r="184" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y183" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z183" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A184" s="1" t="s">
         <v>168</v>
       </c>
@@ -14212,7 +15004,7 @@
       <c r="W184" s="18"/>
       <c r="Y184" s="20"/>
     </row>
-    <row r="185" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
         <v>169</v>
       </c>
@@ -14262,7 +15054,7 @@
       <c r="W185" s="18"/>
       <c r="Y185" s="20"/>
     </row>
-    <row r="186" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
         <v>170</v>
       </c>
@@ -14292,7 +15084,7 @@
       <c r="W186" s="18"/>
       <c r="Y186" s="20"/>
     </row>
-    <row r="187" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A187" s="1" t="s">
         <v>171</v>
       </c>
@@ -14322,7 +15114,7 @@
       <c r="W187" s="18"/>
       <c r="Y187" s="20"/>
     </row>
-    <row r="188" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A188" s="2" t="s">
         <v>172</v>
       </c>
@@ -14386,9 +15178,14 @@
       <c r="X188" s="14">
         <v>56</v>
       </c>
-      <c r="Y188" s="20"/>
-    </row>
-    <row r="189" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y188" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z188" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A189" s="2" t="s">
         <v>173</v>
       </c>
@@ -14460,9 +15257,14 @@
       <c r="X189" s="14">
         <v>108</v>
       </c>
-      <c r="Y189" s="20"/>
-    </row>
-    <row r="190" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y189" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z189" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A190" s="2" t="s">
         <v>174</v>
       </c>
@@ -14534,9 +15336,14 @@
       <c r="X190" s="14">
         <v>74</v>
       </c>
-      <c r="Y190" s="20"/>
-    </row>
-    <row r="191" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y190" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z190" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A191" s="1" t="s">
         <v>175</v>
       </c>
@@ -14566,7 +15373,7 @@
       <c r="W191" s="18"/>
       <c r="Y191" s="20"/>
     </row>
-    <row r="192" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A192" s="1" t="s">
         <v>176</v>
       </c>
@@ -14630,9 +15437,14 @@
       <c r="X192" s="14">
         <v>34</v>
       </c>
-      <c r="Y192" s="20"/>
-    </row>
-    <row r="193" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y192" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A193" s="1" t="s">
         <v>177</v>
       </c>
@@ -14662,7 +15474,7 @@
       <c r="W193" s="18"/>
       <c r="Y193" s="20"/>
     </row>
-    <row r="194" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A194" s="1" t="s">
         <v>178</v>
       </c>
@@ -14734,9 +15546,14 @@
       <c r="X194" s="14">
         <v>118</v>
       </c>
-      <c r="Y194" s="20"/>
-    </row>
-    <row r="195" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y194" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z194" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A195" s="1" t="s">
         <v>179</v>
       </c>
@@ -14813,9 +15630,14 @@
       <c r="X195" s="14">
         <v>110</v>
       </c>
-      <c r="Y195" s="20"/>
-    </row>
-    <row r="196" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y195" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z195" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A196" s="1" t="s">
         <v>180</v>
       </c>
@@ -14887,9 +15709,14 @@
       <c r="X196" s="14">
         <v>146</v>
       </c>
-      <c r="Y196" s="20"/>
-    </row>
-    <row r="197" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y196" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z196" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A197" s="2" t="s">
         <v>181</v>
       </c>
@@ -14966,9 +15793,14 @@
       <c r="X197" s="14">
         <v>190</v>
       </c>
-      <c r="Y197" s="20"/>
-    </row>
-    <row r="198" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y197" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z197" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A198" s="2" t="s">
         <v>182</v>
       </c>
@@ -15040,9 +15872,14 @@
       <c r="X198" s="14">
         <v>128</v>
       </c>
-      <c r="Y198" s="20"/>
-    </row>
-    <row r="199" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y198" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z198" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A199" s="2" t="s">
         <v>183</v>
       </c>
@@ -15114,9 +15951,14 @@
       <c r="X199" s="14">
         <v>146</v>
       </c>
-      <c r="Y199" s="20"/>
-    </row>
-    <row r="200" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y199" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z199" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
         <v>184</v>
       </c>
@@ -15164,7 +16006,7 @@
       <c r="W200" s="18"/>
       <c r="Y200" s="20"/>
     </row>
-    <row r="201" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A201" s="1" t="s">
         <v>185</v>
       </c>
@@ -15241,9 +16083,14 @@
       <c r="X201" s="14">
         <v>162</v>
       </c>
-      <c r="Y201" s="20"/>
-    </row>
-    <row r="202" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y201" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z201" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
         <v>186</v>
       </c>
@@ -15291,7 +16138,7 @@
       <c r="W202" s="18"/>
       <c r="Y202" s="20"/>
     </row>
-    <row r="203" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A203" s="1" t="s">
         <v>187</v>
       </c>
@@ -15363,9 +16210,14 @@
       <c r="X203" s="14">
         <v>132</v>
       </c>
-      <c r="Y203" s="20"/>
-    </row>
-    <row r="204" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y203" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z203" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A204" s="1" t="s">
         <v>188</v>
       </c>
@@ -15427,9 +16279,14 @@
       <c r="X204" s="14">
         <v>40</v>
       </c>
-      <c r="Y204" s="20"/>
-    </row>
-    <row r="205" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y204" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z204" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A205" s="7" t="s">
         <v>189</v>
       </c>
@@ -15482,7 +16339,7 @@
       <c r="W205" s="18"/>
       <c r="Y205" s="20"/>
     </row>
-    <row r="206" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A206" s="1" t="s">
         <v>190</v>
       </c>
@@ -15559,9 +16416,14 @@
       <c r="X206" s="14">
         <v>110</v>
       </c>
-      <c r="Y206" s="20"/>
-    </row>
-    <row r="207" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y206" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z206" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A207" s="1" t="s">
         <v>191</v>
       </c>
@@ -15628,9 +16490,14 @@
       <c r="X207" s="14">
         <v>32</v>
       </c>
-      <c r="Y207" s="20"/>
-    </row>
-    <row r="208" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y207" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z207" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A208" s="1" t="s">
         <v>192</v>
       </c>
@@ -15688,7 +16555,7 @@
       </c>
       <c r="Y208" s="20"/>
     </row>
-    <row r="209" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A209" s="1" t="s">
         <v>193</v>
       </c>
@@ -15757,9 +16624,14 @@
       <c r="X209" s="14">
         <v>12</v>
       </c>
-      <c r="Y209" s="20"/>
-    </row>
-    <row r="210" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y209" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z209" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A210" s="1" t="s">
         <v>194</v>
       </c>
@@ -15823,9 +16695,14 @@
       <c r="X210" s="14">
         <v>40</v>
       </c>
-      <c r="Y210" s="20"/>
-    </row>
-    <row r="211" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y210" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z210" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A211" s="1" t="s">
         <v>195</v>
       </c>
@@ -15902,9 +16779,14 @@
       <c r="X211" s="14">
         <v>8</v>
       </c>
-      <c r="Y211" s="20"/>
-    </row>
-    <row r="212" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y211" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z211" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A212" s="1" t="s">
         <v>196</v>
       </c>
@@ -15934,7 +16816,7 @@
       <c r="W212" s="18"/>
       <c r="Y212" s="20"/>
     </row>
-    <row r="213" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A213" s="1" t="s">
         <v>197</v>
       </c>
@@ -15996,9 +16878,14 @@
       <c r="X213" s="14">
         <v>12</v>
       </c>
-      <c r="Y213" s="20"/>
-    </row>
-    <row r="214" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y213" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z213" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A214" s="1" t="s">
         <v>198</v>
       </c>
@@ -16073,9 +16960,14 @@
       <c r="X214" s="14">
         <v>66</v>
       </c>
-      <c r="Y214" s="20"/>
-    </row>
-    <row r="215" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y214" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z214" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A215" s="1" t="s">
         <v>199</v>
       </c>
@@ -16147,9 +17039,14 @@
       <c r="X215" s="14">
         <v>90</v>
       </c>
-      <c r="Y215" s="20"/>
-    </row>
-    <row r="216" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y215" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z215" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A216" s="1" t="s">
         <v>200</v>
       </c>
@@ -16213,7 +17110,7 @@
       </c>
       <c r="Y216" s="20"/>
     </row>
-    <row r="217" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="s">
         <v>201</v>
       </c>
@@ -16285,9 +17182,14 @@
       <c r="X217" s="14">
         <v>84</v>
       </c>
-      <c r="Y217" s="20"/>
-    </row>
-    <row r="218" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y217" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z217" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A218" s="1" t="s">
         <v>202</v>
       </c>
@@ -16359,9 +17261,14 @@
       <c r="X218" s="14">
         <v>114</v>
       </c>
-      <c r="Y218" s="20"/>
-    </row>
-    <row r="219" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y218" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z218" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A219" s="1" t="s">
         <v>203</v>
       </c>
@@ -16425,9 +17332,14 @@
       <c r="X219" s="14">
         <v>94</v>
       </c>
-      <c r="Y219" s="20"/>
-    </row>
-    <row r="220" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y219" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z219" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A220" s="1" t="s">
         <v>204</v>
       </c>
@@ -16494,9 +17406,14 @@
       <c r="X220" s="14">
         <v>46</v>
       </c>
-      <c r="Y220" s="20"/>
-    </row>
-    <row r="221" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y220" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z220" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A221" s="1" t="s">
         <v>205</v>
       </c>
@@ -16558,9 +17475,14 @@
       <c r="X221" s="14">
         <v>44</v>
       </c>
-      <c r="Y221" s="20"/>
-    </row>
-    <row r="222" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y221" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z221" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A222" s="1" t="s">
         <v>206</v>
       </c>
@@ -16637,9 +17559,14 @@
       <c r="X222" s="14">
         <v>100</v>
       </c>
-      <c r="Y222" s="20"/>
-    </row>
-    <row r="223" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y222" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z222" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A223" s="1" t="s">
         <v>207</v>
       </c>
@@ -16711,9 +17638,14 @@
       <c r="X223" s="14">
         <v>104</v>
       </c>
-      <c r="Y223" s="20"/>
-    </row>
-    <row r="224" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y223" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z223" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A224" s="1" t="s">
         <v>208</v>
       </c>
@@ -16761,7 +17693,7 @@
       <c r="W224" s="18"/>
       <c r="Y224" s="20"/>
     </row>
-    <row r="225" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A225" s="1" t="s">
         <v>209</v>
       </c>
@@ -16838,9 +17770,14 @@
       <c r="X225" s="14">
         <v>140</v>
       </c>
-      <c r="Y225" s="20"/>
-    </row>
-    <row r="226" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y225" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z225" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A226" s="1" t="s">
         <v>210</v>
       </c>
@@ -16888,7 +17825,7 @@
       <c r="W226" s="18"/>
       <c r="Y226" s="20"/>
     </row>
-    <row r="227" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A227" s="1" t="s">
         <v>211</v>
       </c>
@@ -16960,9 +17897,14 @@
       <c r="X227" s="14">
         <v>174</v>
       </c>
-      <c r="Y227" s="20"/>
-    </row>
-    <row r="228" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y227" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z227" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A228" s="1" t="s">
         <v>212</v>
       </c>
@@ -17029,9 +17971,14 @@
       <c r="X228" s="14">
         <v>136</v>
       </c>
-      <c r="Y228" s="20"/>
-    </row>
-    <row r="229" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y228" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z228" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A229" s="1" t="s">
         <v>213</v>
       </c>
@@ -17108,9 +18055,14 @@
       <c r="X229" s="14">
         <v>180</v>
       </c>
-      <c r="Y229" s="20"/>
-    </row>
-    <row r="230" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y229" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z229" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A230" s="1" t="s">
         <v>214</v>
       </c>
@@ -17174,7 +18126,7 @@
       </c>
       <c r="Y230" s="20"/>
     </row>
-    <row r="231" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A231" s="1" t="s">
         <v>215</v>
       </c>
@@ -17238,7 +18190,7 @@
       </c>
       <c r="Y231" s="20"/>
     </row>
-    <row r="232" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A232" s="7" t="s">
         <v>216</v>
       </c>
@@ -17276,7 +18228,7 @@
       </c>
       <c r="Y232" s="20"/>
     </row>
-    <row r="233" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A233" s="1" t="s">
         <v>217</v>
       </c>
@@ -17308,7 +18260,7 @@
       <c r="W233" s="18"/>
       <c r="Y233" s="20"/>
     </row>
-    <row r="234" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A234" s="1" t="s">
         <v>218</v>
       </c>
@@ -17378,9 +18330,14 @@
       <c r="X234" s="14">
         <v>24</v>
       </c>
-      <c r="Y234" s="20"/>
-    </row>
-    <row r="235" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y234" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z234" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A235" s="1" t="s">
         <v>219</v>
       </c>
@@ -17452,9 +18409,14 @@
       <c r="X235" s="14">
         <v>100</v>
       </c>
-      <c r="Y235" s="20"/>
-    </row>
-    <row r="236" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y235" s="20">
+        <v>3</v>
+      </c>
+      <c r="Z235" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A236" s="1" t="s">
         <v>220</v>
       </c>
@@ -17523,9 +18485,14 @@
       <c r="X236" s="14">
         <v>110</v>
       </c>
-      <c r="Y236" s="20"/>
-    </row>
-    <row r="237" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y236" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z236" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A237" s="1" t="s">
         <v>221</v>
       </c>
@@ -17573,7 +18540,7 @@
       </c>
       <c r="Y237" s="20"/>
     </row>
-    <row r="238" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A238" s="1" t="s">
         <v>222</v>
       </c>
@@ -17641,9 +18608,14 @@
       <c r="X238" s="14">
         <v>88</v>
       </c>
-      <c r="Y238" s="20"/>
-    </row>
-    <row r="239" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y238" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z238" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A239" s="3" t="s">
         <v>223</v>
       </c>
@@ -17720,9 +18692,14 @@
       <c r="X239" s="14">
         <v>76</v>
       </c>
-      <c r="Y239" s="20"/>
-    </row>
-    <row r="240" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y239" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z239" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A240" s="3" t="s">
         <v>224</v>
       </c>
@@ -17799,9 +18776,14 @@
       <c r="X240" s="14">
         <v>68</v>
       </c>
-      <c r="Y240" s="20"/>
-    </row>
-    <row r="241" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y240" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z240" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A241" s="3" t="s">
         <v>225</v>
       </c>
@@ -17878,9 +18860,14 @@
       <c r="X241" s="14">
         <v>60</v>
       </c>
-      <c r="Y241" s="20"/>
-    </row>
-    <row r="242" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y241" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z241" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A242" s="1" t="s">
         <v>226</v>
       </c>
@@ -17944,9 +18931,14 @@
       <c r="X242" s="14">
         <v>94</v>
       </c>
-      <c r="Y242" s="20"/>
-    </row>
-    <row r="243" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y242" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z242" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A243" s="1" t="s">
         <v>227</v>
       </c>
@@ -18017,9 +19009,14 @@
       <c r="X243" s="14">
         <v>104</v>
       </c>
-      <c r="Y243" s="20"/>
-    </row>
-    <row r="244" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y243" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z243" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A244" s="1" t="s">
         <v>228</v>
       </c>
@@ -18085,9 +19082,14 @@
       <c r="X244" s="14">
         <v>46</v>
       </c>
-      <c r="Y244" s="20"/>
-    </row>
-    <row r="245" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y244" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z244" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A245" s="1" t="s">
         <v>229</v>
       </c>
@@ -18157,9 +19159,14 @@
       <c r="X245" s="14">
         <v>56</v>
       </c>
-      <c r="Y245" s="20"/>
-    </row>
-    <row r="246" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y245" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z245" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A246" s="1" t="s">
         <v>230</v>
       </c>
@@ -18231,9 +19238,14 @@
       <c r="X246" s="14">
         <v>62</v>
       </c>
-      <c r="Y246" s="20"/>
-    </row>
-    <row r="247" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y246" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z246" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A247" s="1" t="s">
         <v>231</v>
       </c>
@@ -18305,9 +19317,14 @@
       <c r="X247" s="14">
         <v>84</v>
       </c>
-      <c r="Y247" s="20"/>
-    </row>
-    <row r="248" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y247" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z247" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A248" s="1" t="s">
         <v>232</v>
       </c>
@@ -18384,9 +19401,14 @@
       <c r="X248" s="14">
         <v>148</v>
       </c>
-      <c r="Y248" s="20"/>
-    </row>
-    <row r="249" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y248" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z248" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A249" s="1" t="s">
         <v>233</v>
       </c>
@@ -18463,9 +19485,14 @@
       <c r="X249" s="14">
         <v>110</v>
       </c>
-      <c r="Y249" s="20"/>
-    </row>
-    <row r="250" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y249" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z249" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A250" s="1" t="s">
         <v>234</v>
       </c>
@@ -18539,7 +19566,7 @@
       </c>
       <c r="Y250" s="20"/>
     </row>
-    <row r="251" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A251" s="1" t="s">
         <v>235</v>
       </c>
@@ -18563,7 +19590,7 @@
       <c r="W251" s="18"/>
       <c r="Y251" s="20"/>
     </row>
-    <row r="252" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A252" s="12" t="s">
         <v>236</v>
       </c>
@@ -18621,7 +19648,7 @@
       </c>
       <c r="Y252" s="27"/>
     </row>
-    <row r="253" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A253" s="12" t="s">
         <v>237</v>
       </c>
@@ -18679,7 +19706,7 @@
       </c>
       <c r="Y253" s="27"/>
     </row>
-    <row r="254" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A254" s="1" t="s">
         <v>238</v>
       </c>
@@ -18709,7 +19736,7 @@
       <c r="W254" s="18"/>
       <c r="Y254" s="20"/>
     </row>
-    <row r="255" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A255" s="1" t="s">
         <v>239</v>
       </c>
@@ -18757,7 +19784,7 @@
       </c>
       <c r="Y255" s="20"/>
     </row>
-    <row r="256" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A256" s="1" t="s">
         <v>240</v>
       </c>
@@ -18787,7 +19814,7 @@
       <c r="W256" s="18"/>
       <c r="Y256" s="20"/>
     </row>
-    <row r="257" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A257" s="1" t="s">
         <v>241</v>
       </c>
@@ -18858,9 +19885,14 @@
       <c r="X257" s="14">
         <v>116</v>
       </c>
-      <c r="Y257" s="20"/>
-    </row>
-    <row r="258" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y257" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z257" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A258" s="7" t="s">
         <v>242</v>
       </c>
@@ -18909,9 +19941,14 @@
       <c r="X258" s="14">
         <v>26</v>
       </c>
-      <c r="Y258" s="20"/>
-    </row>
-    <row r="259" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y258" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z258" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A259" s="1" t="s">
         <v>243</v>
       </c>
@@ -18978,9 +20015,14 @@
       <c r="X259" s="14">
         <v>58</v>
       </c>
-      <c r="Y259" s="20"/>
-    </row>
-    <row r="260" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y259" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z259" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A260" s="1" t="s">
         <v>244</v>
       </c>
@@ -19010,7 +20052,7 @@
       <c r="W260" s="18"/>
       <c r="Y260" s="20"/>
     </row>
-    <row r="261" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A261" s="1" t="s">
         <v>245</v>
       </c>
@@ -19040,7 +20082,7 @@
       <c r="W261" s="18"/>
       <c r="Y261" s="20"/>
     </row>
-    <row r="262" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A262" s="1" t="s">
         <v>246</v>
       </c>
@@ -19109,9 +20151,14 @@
       <c r="X262" s="14">
         <v>48</v>
       </c>
-      <c r="Y262" s="20"/>
-    </row>
-    <row r="263" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y262" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z262" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A263" s="1" t="s">
         <v>247</v>
       </c>
@@ -19180,9 +20227,14 @@
       <c r="X263" s="14">
         <v>78</v>
       </c>
-      <c r="Y263" s="20"/>
-    </row>
-    <row r="264" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y263" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z263" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A264" s="1" t="s">
         <v>248</v>
       </c>
@@ -19254,9 +20306,14 @@
       <c r="X264" s="14">
         <v>86</v>
       </c>
-      <c r="Y264" s="20"/>
-    </row>
-    <row r="265" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y264" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z264" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A265" s="1" t="s">
         <v>249</v>
       </c>
@@ -19328,9 +20385,14 @@
       <c r="X265" s="14">
         <v>120</v>
       </c>
-      <c r="Y265" s="20"/>
-    </row>
-    <row r="266" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y265" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z265" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A266" s="1" t="s">
         <v>250</v>
       </c>
@@ -19402,9 +20464,14 @@
       <c r="X266" s="14">
         <v>120</v>
       </c>
-      <c r="Y266" s="20"/>
-    </row>
-    <row r="267" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y266" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z266" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A267" s="1" t="s">
         <v>251</v>
       </c>
@@ -19481,9 +20548,14 @@
       <c r="X267" s="14">
         <v>116</v>
       </c>
-      <c r="Y267" s="20"/>
-    </row>
-    <row r="268" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y267" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z267" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A268" s="1" t="s">
         <v>252</v>
       </c>
@@ -19555,9 +20627,14 @@
       <c r="X268" s="14">
         <v>112</v>
       </c>
-      <c r="Y268" s="20"/>
-    </row>
-    <row r="269" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y268" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z268" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A269" s="3" t="s">
         <v>253</v>
       </c>
@@ -19623,9 +20700,14 @@
       <c r="X269" s="14">
         <v>88</v>
       </c>
-      <c r="Y269" s="20"/>
-    </row>
-    <row r="270" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y269" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z269" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A270" s="3" t="s">
         <v>254</v>
       </c>
@@ -19697,9 +20779,14 @@
       <c r="X270" s="14">
         <v>82</v>
       </c>
-      <c r="Y270" s="20"/>
-    </row>
-    <row r="271" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y270" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z270" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A271" s="3" t="s">
         <v>255</v>
       </c>
@@ -19771,9 +20858,14 @@
       <c r="X271" s="14">
         <v>82</v>
       </c>
-      <c r="Y271" s="20"/>
-    </row>
-    <row r="272" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y271" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z271" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A272" s="1" t="s">
         <v>256</v>
       </c>
@@ -19845,9 +20937,14 @@
       <c r="X272" s="14">
         <v>60</v>
       </c>
-      <c r="Y272" s="20"/>
-    </row>
-    <row r="273" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y272" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z272" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A273" s="1" t="s">
         <v>257</v>
       </c>
@@ -19916,9 +21013,14 @@
       <c r="X273" s="14">
         <v>36</v>
       </c>
-      <c r="Y273" s="20"/>
-    </row>
-    <row r="274" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y273" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z273" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="274" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A274" s="1" t="s">
         <v>258</v>
       </c>
@@ -19993,9 +21095,14 @@
       <c r="X274" s="14">
         <v>56</v>
       </c>
-      <c r="Y274" s="20"/>
-    </row>
-    <row r="275" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y274" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z274" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A275" s="1" t="s">
         <v>259</v>
       </c>
@@ -20067,9 +21174,14 @@
       <c r="X275" s="14">
         <v>86</v>
       </c>
-      <c r="Y275" s="20"/>
-    </row>
-    <row r="276" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y275" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z275" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A276" s="1" t="s">
         <v>260</v>
       </c>
@@ -20117,7 +21229,7 @@
       </c>
       <c r="Y276" s="20"/>
     </row>
-    <row r="277" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A277" s="1" t="s">
         <v>261</v>
       </c>
@@ -20183,7 +21295,7 @@
       </c>
       <c r="Y277" s="20"/>
     </row>
-    <row r="278" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A278" s="1" t="s">
         <v>262</v>
       </c>
@@ -20253,9 +21365,14 @@
       <c r="X278" s="14">
         <v>78</v>
       </c>
-      <c r="Y278" s="20"/>
-    </row>
-    <row r="279" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y278" s="20">
+        <v>2</v>
+      </c>
+      <c r="Z278" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A279" s="1" t="s">
         <v>263</v>
       </c>
@@ -20285,7 +21402,7 @@
       <c r="W279" s="18"/>
       <c r="Y279" s="20"/>
     </row>
-    <row r="280" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A280" s="7" t="s">
         <v>264</v>
       </c>
@@ -20322,7 +21439,7 @@
       </c>
       <c r="Y280" s="20"/>
     </row>
-    <row r="281" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A281" s="3" t="s">
         <v>265</v>
       </c>
@@ -20399,9 +21516,14 @@
       <c r="X281" s="14">
         <v>28</v>
       </c>
-      <c r="Y281" s="20"/>
-    </row>
-    <row r="282" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y281" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z281" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A282" s="3" t="s">
         <v>266</v>
       </c>
@@ -20478,9 +21600,14 @@
       <c r="X282" s="14">
         <v>110</v>
       </c>
-      <c r="Y282" s="20"/>
-    </row>
-    <row r="283" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y282" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z282" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A283" s="3" t="s">
         <v>267</v>
       </c>
@@ -20557,9 +21684,14 @@
       <c r="X283" s="14">
         <v>80</v>
       </c>
-      <c r="Y283" s="20"/>
-    </row>
-    <row r="284" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Y283" s="20">
+        <v>1</v>
+      </c>
+      <c r="Z283" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A284" s="5" t="s">
         <v>268</v>
       </c>
@@ -20636,9 +21768,14 @@
       <c r="X284" s="50">
         <v>136</v>
       </c>
-      <c r="Y284" s="25"/>
-    </row>
-    <row r="287" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Y284" s="25">
+        <v>2</v>
+      </c>
+      <c r="Z284" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287" spans="1:26" x14ac:dyDescent="0.35">
       <c r="J287" s="10"/>
       <c r="L287" s="10"/>
       <c r="M287" s="10"/>

</xml_diff>